<commit_message>
Added dataset mapping functions
</commit_message>
<xml_diff>
--- a/data-raw/controlled_vocab_mapping.xlsx
+++ b/data-raw/controlled_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9041DB46-C88C-4313-B089-F8FBE4349FF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EED1E9-48EC-4768-BD90-FD91403D13F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86950A22-EF96-470E-9EC4-A018FD5DBEF2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="501">
   <si>
     <t>machine_name</t>
   </si>
@@ -1509,6 +1509,30 @@
   </si>
   <si>
     <t>FALSE</t>
+  </si>
+  <si>
+    <t>CC0</t>
+  </si>
+  <si>
+    <t>CC0 1.0</t>
+  </si>
+  <si>
+    <t>Creative Commons Attribution 4.0</t>
+  </si>
+  <si>
+    <t>Creative Commons Attribution-NonCommercial 4.0</t>
+  </si>
+  <si>
+    <t>Creative Commons Attribution Share-Alike 4.0</t>
+  </si>
+  <si>
+    <t>Open Database License</t>
+  </si>
+  <si>
+    <t>Open Data Commons Open Database License 1.0</t>
+  </si>
+  <si>
+    <t>field_license_wbddh</t>
   </si>
 </sst>
 </file>
@@ -1576,12 +1600,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1898,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C28C184-6D7E-43FA-B606-BF9631A08DC0}">
-  <dimension ref="A1:D269"/>
+  <dimension ref="A1:D274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258:XFD258"/>
+      <selection activeCell="I269" sqref="I269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5599,6 +5626,76 @@
         <v>492</v>
       </c>
     </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>500</v>
+      </c>
+      <c r="B270" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C270" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="D270" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>500</v>
+      </c>
+      <c r="B271" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="D271" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>500</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="D272" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>500</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C273" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="D273" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>500</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="D274" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cleaned code and added functionality to add invalid country codes to external metadata
</commit_message>
<xml_diff>
--- a/data-raw/controlled_vocab_mapping.xlsx
+++ b/data-raw/controlled_vocab_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CC7B4F-21A3-4765-A9F2-CA5D715D6EDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98782743-D6E1-4F15-96DD-AAEEC2A01C75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86950A22-EF96-470E-9EC4-A018FD5DBEF2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="464">
   <si>
     <t>machine_name</t>
   </si>
@@ -1356,105 +1356,6 @@
   </si>
   <si>
     <t>Region/Country not specified</t>
-  </si>
-  <si>
-    <t>AIA</t>
-  </si>
-  <si>
-    <t>ALA</t>
-  </si>
-  <si>
-    <t>ATA</t>
-  </si>
-  <si>
-    <t>ATF</t>
-  </si>
-  <si>
-    <t>BES</t>
-  </si>
-  <si>
-    <t>BLM</t>
-  </si>
-  <si>
-    <t>BVT</t>
-  </si>
-  <si>
-    <t>CCK</t>
-  </si>
-  <si>
-    <t>COK</t>
-  </si>
-  <si>
-    <t>CXR</t>
-  </si>
-  <si>
-    <t>ESH</t>
-  </si>
-  <si>
-    <t>FLK</t>
-  </si>
-  <si>
-    <t>GGY</t>
-  </si>
-  <si>
-    <t>GLP</t>
-  </si>
-  <si>
-    <t>GUF</t>
-  </si>
-  <si>
-    <t>HMD</t>
-  </si>
-  <si>
-    <t>IOT</t>
-  </si>
-  <si>
-    <t>JEY</t>
-  </si>
-  <si>
-    <t>MSR</t>
-  </si>
-  <si>
-    <t>MTQ</t>
-  </si>
-  <si>
-    <t>MYT</t>
-  </si>
-  <si>
-    <t>NFK</t>
-  </si>
-  <si>
-    <t>NIU</t>
-  </si>
-  <si>
-    <t>PCN</t>
-  </si>
-  <si>
-    <t>REU</t>
-  </si>
-  <si>
-    <t>SGS</t>
-  </si>
-  <si>
-    <t>SHN</t>
-  </si>
-  <si>
-    <t>SJM</t>
-  </si>
-  <si>
-    <t>SPM</t>
-  </si>
-  <si>
-    <t>TKL</t>
-  </si>
-  <si>
-    <t>UMI</t>
-  </si>
-  <si>
-    <t>VAT</t>
-  </si>
-  <si>
-    <t>WLF</t>
   </si>
   <si>
     <t>list_value_name</t>
@@ -1907,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C28C184-6D7E-43FA-B606-BF9631A08DC0}">
-  <dimension ref="A1:D272"/>
+  <dimension ref="A1:D239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268:XFD268"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="H220" sqref="H220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,13 +1826,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>476</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5029,630 +4930,168 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B223" t="s">
-        <v>441</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="D223" t="b">
-        <v>1</v>
+      <c r="A223" t="s">
+        <v>444</v>
+      </c>
+      <c r="D223" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B224" t="s">
-        <v>441</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="D224" t="b">
-        <v>1</v>
+      <c r="A224" t="s">
+        <v>445</v>
+      </c>
+      <c r="D224" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B225" t="s">
-        <v>441</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="D225" t="b">
-        <v>1</v>
+      <c r="A225" t="s">
+        <v>446</v>
+      </c>
+      <c r="D225" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B226" t="s">
-        <v>441</v>
-      </c>
-      <c r="C226" s="3" t="s">
+      <c r="A226" t="s">
+        <v>447</v>
+      </c>
+      <c r="D226" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>448</v>
+      </c>
+      <c r="D227" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>449</v>
+      </c>
+      <c r="D228" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>450</v>
+      </c>
+      <c r="D229" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>451</v>
+      </c>
+      <c r="D230" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>452</v>
+      </c>
+      <c r="D231" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>453</v>
+      </c>
+      <c r="D232" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>446</v>
+      </c>
+      <c r="D233" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>445</v>
       </c>
-      <c r="D226" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B227" t="s">
-        <v>441</v>
-      </c>
-      <c r="C227" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="D227" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B228" t="s">
-        <v>441</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="D228" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B229" t="s">
-        <v>441</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="D229" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B230" t="s">
-        <v>441</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="D230" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B231" t="s">
-        <v>441</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="D231" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B232" t="s">
-        <v>441</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="D232" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B233" t="s">
-        <v>441</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="D233" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B234" t="s">
-        <v>441</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D234" t="b">
-        <v>1</v>
+      <c r="D234" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B235" t="s">
-        <v>441</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>454</v>
+      <c r="A235" t="s">
+        <v>463</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>457</v>
       </c>
       <c r="D235" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B236" t="s">
-        <v>441</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>455</v>
+      <c r="A236" t="s">
+        <v>463</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>458</v>
       </c>
       <c r="D236" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" t="s">
-        <v>441</v>
-      </c>
-      <c r="C237" s="3" t="s">
-        <v>456</v>
+    <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>463</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>459</v>
       </c>
       <c r="D237" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B238" t="s">
-        <v>441</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>457</v>
+      <c r="A238" t="s">
+        <v>463</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>460</v>
       </c>
       <c r="D238" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B239" t="s">
-        <v>441</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>458</v>
+    <row r="239" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>463</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>462</v>
       </c>
       <c r="D239" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B240" t="s">
-        <v>441</v>
-      </c>
-      <c r="C240" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="D240" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B241" t="s">
-        <v>441</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="D241" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B242" t="s">
-        <v>441</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="D242" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B243" t="s">
-        <v>441</v>
-      </c>
-      <c r="C243" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="D243" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B244" t="s">
-        <v>441</v>
-      </c>
-      <c r="C244" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="D244" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B245" t="s">
-        <v>441</v>
-      </c>
-      <c r="C245" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="D245" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B246" t="s">
-        <v>441</v>
-      </c>
-      <c r="C246" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="D246" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B247" t="s">
-        <v>441</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="D247" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B248" t="s">
-        <v>441</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="D248" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B249" t="s">
-        <v>441</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="D249" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B250" t="s">
-        <v>441</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="D250" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B251" t="s">
-        <v>441</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="D251" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B252" t="s">
-        <v>441</v>
-      </c>
-      <c r="C252" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="D252" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B253" t="s">
-        <v>441</v>
-      </c>
-      <c r="C253" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="D253" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B254" t="s">
-        <v>441</v>
-      </c>
-      <c r="C254" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="D254" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B255" t="s">
-        <v>441</v>
-      </c>
-      <c r="C255" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="D255" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>477</v>
-      </c>
-      <c r="D256" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>478</v>
-      </c>
-      <c r="D257" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>479</v>
-      </c>
-      <c r="D258" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>480</v>
-      </c>
-      <c r="D259" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>481</v>
-      </c>
-      <c r="D260" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>482</v>
-      </c>
-      <c r="D261" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>483</v>
-      </c>
-      <c r="D262" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>484</v>
-      </c>
-      <c r="D263" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>485</v>
-      </c>
-      <c r="D264" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>486</v>
-      </c>
-      <c r="D265" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>479</v>
-      </c>
-      <c r="D266" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>478</v>
-      </c>
-      <c r="D267" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>496</v>
-      </c>
-      <c r="B268" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="C268" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="D268" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>496</v>
-      </c>
-      <c r="B269" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="C269" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="D269" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>496</v>
-      </c>
-      <c r="B270" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="C270" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="D270" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>496</v>
-      </c>
-      <c r="B271" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C271" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="D271" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>496</v>
-      </c>
-      <c r="B272" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="C272" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="D272" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>